<commit_message>
feat: add new sinead request cell line filters
Signed-off-by: Ali Sajid Imami <395482+AliSajid@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/results/cell-line-exploration/triple_ranked_comparisons.xlsx
+++ b/results/cell-line-exploration/triple_ranked_comparisons.xlsx
@@ -1281,7 +1281,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>HA1E-24h-10uM</t>
+          <t>ASC-24h-10uM</t>
         </is>
       </c>
       <c r="B33">
@@ -1294,7 +1294,7 @@
         <v>1</v>
       </c>
       <c r="E33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F33">
         <v>2</v>
@@ -1303,41 +1303,41 @@
         <v>1</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>OV7-6h-10uM</t>
+          <t>HA1E-24h-10uM</t>
         </is>
       </c>
       <c r="B34">
         <v>1.666666666666667</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F34">
         <v>2</v>
       </c>
       <c r="G34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>SW620-6h-10uM</t>
+          <t>OV7-6h-10uM</t>
         </is>
       </c>
       <c r="B35">
@@ -1350,22 +1350,22 @@
         <v>1</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F35">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>YAPC-24h-0.37uM</t>
+          <t>SW620-6h-10uM</t>
         </is>
       </c>
       <c r="B36">
@@ -1378,10 +1378,10 @@
         <v>1</v>
       </c>
       <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
         <v>5</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -1393,29 +1393,29 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ASC-24h-10uM</t>
+          <t>YAPC-24h-0.37uM</t>
         </is>
       </c>
       <c r="B37">
-        <v>1.833333333333333</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G37">
         <v>1</v>
       </c>
       <c r="H37">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">

</xml_diff>